<commit_message>
P7 subprogram (shoulnd't be in master)
last time I went to hell switching to PRg7... I'll do it soon with care
</commit_message>
<xml_diff>
--- a/Patent2Net/Resources/EntitésPubliquesNorm4.xlsx
+++ b/Patent2Net/Resources/EntitésPubliquesNorm4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AnacondaProjects\P2N-der\Patent2Net\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AnacondaProjects\P2N-v3\Patent2Net\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D93F8E-868C-4C7B-9763-5135A3C61D6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA433B0-F5E5-43FD-AD71-D6C6D49325F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8355" yWindow="7695" windowWidth="23550" windowHeight="13785" tabRatio="678" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="2100" windowWidth="27135" windowHeight="13890" tabRatio="678" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Univ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2963" uniqueCount="2946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="2947">
   <si>
     <t>Univ</t>
   </si>
@@ -8863,6 +8863,9 @@
   </si>
   <si>
     <t>UNIV HUAZHONG</t>
+  </si>
+  <si>
+    <t>CHU PARIS</t>
   </si>
 </sst>
 </file>
@@ -23768,10 +23771,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23929,6 +23932,11 @@
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2946</v>
       </c>
     </row>
   </sheetData>
@@ -23940,8 +23948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>